<commit_message>
Modificaciones en DebinQR 2
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A51162-926E-4942-A8C3-960E1DB451EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FF8294-DDC3-4D31-8015-4ACDAF011E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="124">
   <si>
     <t>Parametros</t>
   </si>
@@ -399,6 +399,12 @@
   </si>
   <si>
     <t>"operacion":{"vendedor": {"cbu": "9980001100000000000017",}}</t>
+  </si>
+  <si>
+    <t>ID USUARIO INVALIDO</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo": "","descripcion": "MONEDA INEXISTENTE"}}}</t>
   </si>
 </sst>
 </file>
@@ -758,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1102,7 +1108,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1113,7 +1119,7 @@
         <v>77</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>123</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>48</v>
@@ -1337,7 +1343,7 @@
         <v>83</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
ID en Archivo DebinQR
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9FD34CD-6624-4450-A3A6-02D0CB9B2054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF33E75A-C2BE-4D51-9D33-DDF15490EEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1665" yWindow="2040" windowWidth="11310" windowHeight="7875" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR" sheetId="7" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>CBU MAL FORMULADO COMPRADOR</t>
   </si>
   <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo": "","descripcion": "CBU MAL FORMULADO COMPRADOR"}}}</t>
-  </si>
-  <si>
     <t>CUIT MAL FORMULADO DEL VENDEDOR</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>MONEDA COMPRADOR INCORRECTA</t>
+  </si>
+  <si>
+    <t>"operacion":{"comprador": {"cuenta": {"cbu": "","alias": "null"},"cuit": "27375575847"},}</t>
   </si>
 </sst>
 </file>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -879,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -896,7 +896,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -913,7 +913,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -930,7 +930,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
@@ -947,7 +947,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>23</v>
@@ -970,29 +970,29 @@
         <v>25</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>53808</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>123</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>53809</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>53810</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>5</v>
@@ -1018,9 +1018,9 @@
         <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1032,13 +1032,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1049,13 +1049,13 @@
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1066,13 +1066,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1086,10 +1086,10 @@
         <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1100,13 +1100,13 @@
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1117,13 +1117,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1134,13 +1134,13 @@
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1151,13 +1151,13 @@
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1168,13 +1168,13 @@
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1185,13 +1185,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1202,13 +1202,13 @@
         <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1219,13 +1219,13 @@
         <v>5</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1236,13 +1236,13 @@
         <v>5</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1253,13 +1253,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1270,13 +1270,13 @@
         <v>5</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1287,13 +1287,13 @@
         <v>5</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1304,13 +1304,13 @@
         <v>5</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1321,13 +1321,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1338,13 +1338,13 @@
         <v>5</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1355,13 +1355,13 @@
         <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1372,13 +1372,13 @@
         <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1389,13 +1389,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="E36" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1406,13 +1406,13 @@
         <v>5</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1423,13 +1423,13 @@
         <v>5</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1440,13 +1440,13 @@
         <v>5</v>
       </c>
       <c r="C39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1457,13 +1457,13 @@
         <v>5</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1474,13 +1474,13 @@
         <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="6" t="s">
         <v>104</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1491,13 +1491,13 @@
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1508,13 +1508,13 @@
         <v>5</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1525,13 +1525,13 @@
         <v>5</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1542,13 +1542,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1559,13 +1559,13 @@
         <v>5</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1576,13 +1576,13 @@
         <v>5</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integracion de cambios de debinqr
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF33E75A-C2BE-4D51-9D33-DDF15490EEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEF2C62-EAC8-4272-97CF-65EE51111392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="2040" windowWidth="11310" windowHeight="7875" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR" sheetId="7" r:id="rId1"/>
@@ -776,20 +776,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="54.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -806,7 +806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -820,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>53799</v>
       </c>
@@ -837,7 +837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>53800</v>
       </c>
@@ -854,7 +854,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>53801</v>
       </c>
@@ -871,7 +871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>53802</v>
       </c>
@@ -888,7 +888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>53803</v>
       </c>
@@ -905,7 +905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>53804</v>
       </c>
@@ -922,7 +922,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>53805</v>
       </c>
@@ -939,7 +939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>53806</v>
       </c>
@@ -956,7 +956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>53807</v>
       </c>
@@ -973,7 +973,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>53808</v>
       </c>
@@ -990,7 +990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>53809</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>53810</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
cambios pequeños archivo QR
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7890017-7CD7-4B14-B435-1A640B6731B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0734F478-AD31-4A2F-A4E8-69AB35AF3349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="151">
   <si>
     <t>Parametros</t>
   </si>
@@ -480,16 +480,13 @@
     <t>"operacion_original":{"detalle":{"importe":127},"vendedor":{"cuit":"20333048494","cbu":"0000004800000000008622"},"qr_id_trx":"0060914262123991246"},"objeto":{"ori_trx_id":"00000322"}}</t>
   </si>
   <si>
-    <t xml:space="preserve">Devolución Parcial - ORI_ID_TRX - Parcial con ORI_ID_TRX después de Parcial sin ORI_ID_TRX </t>
-  </si>
-  <si>
     <t>QRSolicitudContraCargo*-&gt;QRSolicitudContraCargo*-&gt;QRSolicitudContraCargo*</t>
   </si>
   <si>
     <t>"operacion_original":{"detalle":{"importe":1},"vendedor":{"cuit":"20333048494","cbu":"0000004800000000008622"},"qr_id_trx":"0060914262123991254"}}|"operacion_original":{"detalle":{"importe":1},"vendedor":{"cuit":"20333048494","cbu":"0000004800000000008622"},"qr_id_trx":"0060914262123991254"}}|"operacion_original":{"detalle":{"importe":1},"vendedor":{"cuit":"20333048494","cbu":"0000004800000000008622"},"qr_id_trx":"0060914262123991254"}}</t>
   </si>
   <si>
-    <t>"operacion_original":{"detalle":{"importe":1},"vendedor":{"cuit":"20333048494","cbu":"0000004800000000008622"},"qr_id_trx":"0060914262123991255"}}|"operacion_original":{"detalle":{"importe":1},"vendedor":{"cuit":"20333048494","cbu":"0000004800000000008622"},"qr_id_trx":"0060914262123991255"}}|"operacion_original":{"detalle":{"importe":1},"vendedor":{"cuit":"20333048494","cbu":"0000004800000000008622"},"qr_id_trx":"0060914262123991255"}}</t>
+    <t xml:space="preserve">Devolución Parcial - ORI_ID_TRX - Parcial con ORI_ID_TRX después de Parcial con ORI_ID_TRX </t>
   </si>
 </sst>
 </file>
@@ -837,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,33 +1738,16 @@
         <v>60906</v>
       </c>
       <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>60907</v>
-      </c>
-      <c r="B54" t="s">
-        <v>149</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pequeño cambio en msj de respuesta
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95AA216-CEAA-43E4-A6E1-E5E54064A6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27112675-BD71-4404-A0D7-F3DD8044A37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,7 +525,7 @@
     <t>QRConfimaDebito - Caso Feliz - Interoperable - Coelsa Aceptador</t>
   </si>
   <si>
-    <t>{"StatusCode":201,"Mensaje":{"respuesta": {"code":"APPROVED","descripcion":"PAYMENT CREACION CORRECTA"}}}</t>
+    <t>{"StatusCode":201,"Mensaje":{"transaction": {"code":"APPROVED","description":"PAYMENT CREACION CORRECTA"}}}</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
cambios de casos fallidos
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{710608BC-3C38-400C-AE3A-2BF9175345D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C7419C-5602-4692-8995-7B13D071CBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2110,7 +2110,7 @@
         <v>60909</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
Validacion parametro de bd
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D712D367-B012-46C8-B72F-52F04E777493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342AD427-B533-42ED-8CB3-8E3F31DE1C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR" sheetId="7" r:id="rId1"/>
@@ -730,22 +730,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -754,12 +745,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1088,58 +1073,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
         <v>53766</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>53799</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1152,14 +1137,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>53800</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1169,14 +1154,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>53801</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>131</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1186,14 +1171,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>53802</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
         <v>135</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1203,14 +1188,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>53803</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>129</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1220,14 +1205,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>53804</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>130</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1237,14 +1222,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>53805</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="3" t="s">
         <v>113</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1254,62 +1239,62 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>53806</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
         <v>132</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>53807</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>53808</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13">
         <v>53809</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1318,15 +1303,15 @@
       <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14">
         <v>53810</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1335,11 +1320,11 @@
       <c r="D14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>53811</v>
       </c>
@@ -1356,11 +1341,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>53812</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1369,49 +1354,49 @@
       <c r="D16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17">
         <v>53813</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18">
         <v>53814</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>53816</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1420,334 +1405,334 @@
       <c r="D19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>53817</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>53818</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
         <v>82</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>53819</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>53820</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
         <v>81</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>53821</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>53822</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
         <v>79</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>53823</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
         <v>76</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>53824</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
         <v>45</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28">
         <v>53825</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29">
         <v>53826</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>78</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30">
         <v>53827</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>53828</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
         <v>72</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32">
         <v>53829</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33">
         <v>53830</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A34">
         <v>53831</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35">
         <v>53832</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36">
         <v>53833</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37">
         <v>53834</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38">
         <v>53835</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>53836</v>
       </c>
@@ -1764,7 +1749,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>53837</v>
       </c>
@@ -1781,42 +1766,42 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41">
         <v>53840</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>96</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42">
         <v>53842</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43">
         <v>59833</v>
       </c>
       <c r="B43" t="s">
@@ -1832,93 +1817,93 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A44">
         <v>59841</v>
       </c>
-      <c r="B44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="7" t="s">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>62080</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="4" t="s">
         <v>164</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>60688</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" t="s">
         <v>167</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="1" t="s">
         <v>166</v>
       </c>
       <c r="E46" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47">
         <v>60780</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" t="s">
         <v>167</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+    <row r="48" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A48">
         <v>59692</v>
       </c>
-      <c r="B48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="7" t="s">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>209</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+    <row r="49" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A49">
         <v>59693</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="7" t="s">
+      <c r="B49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>210</v>
       </c>
       <c r="D49" s="2" t="s">
@@ -1928,14 +1913,14 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+    <row r="50" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A50">
         <v>59695</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="7" t="s">
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>208</v>
       </c>
       <c r="D50" s="2" t="s">
@@ -1945,20 +1930,20 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+    <row r="51" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A51">
         <v>59696</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="7" t="s">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>211</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" t="s">
         <v>212</v>
       </c>
     </row>
@@ -1975,44 +1960,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F88D94-F9F2-4FF5-8669-E80BF5785B88}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>60532</v>
       </c>
       <c r="B2" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>175</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2022,139 +2007,139 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>60902</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>176</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>60903</v>
       </c>
       <c r="B4" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>175</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>60904</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>60905</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
         <v>60906</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>60908</v>
       </c>
       <c r="B8" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>177</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9">
         <v>60909</v>
       </c>
       <c r="B9" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="4" t="s">
         <v>178</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10">
         <v>60910</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="5" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2168,84 +2153,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13F07D4-A043-4E09-992B-E3E60FFD6B6A}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>59007</v>
       </c>
       <c r="B2" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>128</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>59006</v>
       </c>
       <c r="B3" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="4" t="s">
         <v>125</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>59305</v>
       </c>
       <c r="B4" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>121</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="5" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2263,59 +2248,58 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>61353</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
         <v>60848</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="16" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="9" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2333,34 +2317,34 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>62551</v>
       </c>
       <c r="B2" t="s">
@@ -2370,11 +2354,11 @@
         <v>174</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>62851</v>
       </c>
@@ -2388,7 +2372,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>62852</v>
       </c>
@@ -2402,7 +2386,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>62854</v>
       </c>
@@ -2412,14 +2396,14 @@
       <c r="C5" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>188</v>
       </c>
       <c r="E5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>59716</v>
       </c>
@@ -2433,7 +2417,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>59718</v>
       </c>
@@ -2447,7 +2431,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>59720</v>
       </c>
@@ -2457,14 +2441,14 @@
       <c r="C8" t="s">
         <v>185</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="5" t="s">
         <v>188</v>
       </c>
       <c r="E8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>53394</v>
       </c>
@@ -2478,21 +2462,21 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>53395</v>
       </c>
       <c r="B10" t="s">
         <v>198</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="4" t="s">
         <v>200</v>
       </c>
       <c r="E10" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>59542</v>
       </c>
@@ -2506,7 +2490,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>59545</v>
       </c>
@@ -2520,7 +2504,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>59551</v>
       </c>
@@ -2530,7 +2514,7 @@
       <c r="C13" t="s">
         <v>185</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="5" t="s">
         <v>188</v>
       </c>
       <c r="E13" t="s">
@@ -2551,71 +2535,71 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+    <row r="2" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>61353</v>
       </c>
       <c r="B2" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="4" t="s">
         <v>170</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>60848</v>
       </c>
       <c r="B3" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="1"/>
       <c r="E3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>60851</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="4"/>
       <c r="E4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>60852</v>
       </c>
@@ -2623,7 +2607,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>60854</v>
       </c>
@@ -2631,7 +2615,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>60955</v>
       </c>
@@ -2639,7 +2623,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>61946</v>
       </c>

</xml_diff>

<commit_message>
Validacion de parametro bd
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342AD427-B533-42ED-8CB3-8E3F31DE1C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981238D1-0E67-4561-88B1-E44F0596D565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR" sheetId="7" r:id="rId1"/>
@@ -18,14 +18,12 @@
     <sheet name="CASHOUT" sheetId="9" r:id="rId3"/>
     <sheet name="INTEROPERBILIDAD" sheetId="12" r:id="rId4"/>
     <sheet name="GETs" sheetId="13" r:id="rId5"/>
-    <sheet name="INTEROPERBILIDAD 3" sheetId="10" state="hidden" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CASHOUT!$A$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CONTRACARGOQR!$A$1:$E$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">GETs!$A$1:$E$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">INTEROPERBILIDAD!$A$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'INTEROPERBILIDAD 3'!$A$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">QR!$A$1:$E$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="214">
   <si>
     <t>Parametros</t>
   </si>
@@ -511,18 +509,6 @@
     <t>Interoperable- MVP1 - QRIntencionPago - Caso OK - Datos POST [PSP]/QRIntencionDePago</t>
   </si>
   <si>
-    <t>Interoperable- MVP1 - QRIntencionPago - Caso OK - Envio POST [PSP]/QRIntencionDePago</t>
-  </si>
-  <si>
-    <t>Interoperable- MVP1 - QRIntencionPago - Caso OK - Respuesta QRIntenciondePago</t>
-  </si>
-  <si>
-    <t>Interoperable- MVP1 - QRIntencionPago - Caso OK - Datos Respuesta</t>
-  </si>
-  <si>
-    <t>QRDebin - MVP1 - QRIntencionPago - Caso OK - Datos Respuesta</t>
-  </si>
-  <si>
     <t>QRDebin- MVP1 - QRIntencionPago - Caso OK - Envio POST [PSP]/QRIntencionDePago</t>
   </si>
   <si>
@@ -541,24 +527,15 @@
     <t>"operacion":{"detalle":{"concepto":"VAR","importe":1000}}}</t>
   </si>
   <si>
-    <t>Split - Interoperable - Coelsa Aceptador</t>
-  </si>
-  <si>
     <t>"endpoint":"debin","id":"debin.id","aviso":"QRIntencionPago","producto":"responder"</t>
   </si>
   <si>
     <t>QRDebin-&gt;aviso*</t>
   </si>
   <si>
-    <t>PaymentValidation-&gt;Payment-&gt;aviso*</t>
-  </si>
-  <si>
     <t>PaymentValidation-&gt;Payment</t>
   </si>
   <si>
-    <t>"payer":{"identification_number":"20000000222","document":{"type":"DNI","number":"00000022"},"account":{"cbu":"9981522200000000000192","wallet":{"name":"PAYPAUL","cuit":"20000000346"}},"acquirer":{"reverse_domain":"com.mercadolibre","cuit":"30703088534"},"merchant":{"cuit":"20374372689","account":{"cbu":"0168888100008273570145","cvu":"0000084000000000000024"}}}}|"payer":{"identification_number":"20000000222","document":{"type":"DNI","number":"00000022"},"account":{"cbu":"9981522200000000000192","wallet":{"name":"PAYPAUL","cuit":"20000000346"}},"acquirer":{"reverse_domain":"com.mercadolibre","cuit":"30703088534"},"merchant":{"cuit":"20374372689","account":{"cbu":"0168888100008273570145","cvu":"0000084000000000000024"}}}}|"id":"debin.id","aviso":"QRIntencionPago","producto":"responder"</t>
-  </si>
-  <si>
     <t>PaymentValidation-&gt;aviso*</t>
   </si>
   <si>
@@ -577,15 +554,6 @@
     <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"operacion_original":{"detalle":{"importe":1000}}}</t>
   </si>
   <si>
-    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"operacion_original":{"detalle":{"importe":1},"qr_id_trx":"00000000000111111111111"}}</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"operacion_original":{"detalle":{"importe":1000},"qr_id_trx":"00000000000111111111111"}}</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"operacion_original":{"detalle":{"importe":1}},"objeto":{"ori_trx_id":" "}}</t>
-  </si>
-  <si>
     <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"operacion_original":{"detalle":{"importe":1}}}|"operacion_original":{"detalle":{"importe":1}}}|"operacion_original":{"detalle":{"importe":1}}}</t>
   </si>
   <si>
@@ -683,6 +651,39 @@
   </si>
   <si>
     <t>Nuevo circuito: Cambios /QRDebin - Nuevo campo CUIT Administrador - Cuit Valido</t>
+  </si>
+  <si>
+    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;QRSolicitudContraCargo*-&gt;aviso*</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"operacion_original":{"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"QROperacionFinalizada","producto":"responder"</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"operacion_original":{"detalle":{"importe":250}}}|"id":"debin.id","aviso":"QROperacionFinalizada","producto":"responder"</t>
+  </si>
+  <si>
+    <t>POST [epBilletera]/QROperacionFinalizada - 5705 DEVOLUCION TOTAL (Coelsa - Coelsa)</t>
+  </si>
+  <si>
+    <t>POST [epBilletera]/QROperacionFinalizada - 5708 DEVOLUCION PARCIAL (Coelsa-Coelsa)</t>
+  </si>
+  <si>
+    <t>"id":"4XJ8G7V95JLW86R9EMPYR0"</t>
+  </si>
+  <si>
+    <t>GET Debin4: Propiedad ori_trx_id - Coelsa Coelsa - OK</t>
+  </si>
+  <si>
+    <t>GET Debin4: Propiedad ori_trx_id - Coelsa Billetera - OK</t>
+  </si>
+  <si>
+    <t>"operacion_original":{"detalle":{"importe":1},"qr_id_trx":"00000000000111111111111"},"objeto":{"ori_trx_id":"9223000000000066307"},"sql":"off"</t>
+  </si>
+  <si>
+    <t>"operacion_original":{"detalle":{"importe":1000},"qr_id_trx":"00000000000111111111111"},"objeto":{"ori_trx_id":"9223000000000066307"},"sql":"off"</t>
+  </si>
+  <si>
+    <t>"operacion_original":{"detalle":{"importe":1},"qr_id_trx":"Test%20Auto%2014594309"},"objeto":{"ori_trx_id":" "}},"sql":"off"</t>
   </si>
 </sst>
 </file>
@@ -730,13 +731,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -745,6 +755,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -764,27 +780,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1073,58 +1069,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
         <v>53766</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>53799</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1137,14 +1133,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>53800</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1154,14 +1150,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>53801</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>131</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -1171,14 +1167,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>53802</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1188,14 +1184,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>53803</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>129</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1205,14 +1201,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>53804</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>130</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1222,14 +1218,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>53805</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="8" t="s">
         <v>113</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1239,62 +1235,62 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>53806</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="11" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>53807</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>53808</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>53809</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1303,15 +1299,15 @@
       <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>53810</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1320,11 +1316,11 @@
       <c r="D14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>53811</v>
       </c>
@@ -1341,11 +1337,11 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>53812</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1354,49 +1350,49 @@
       <c r="D16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>53813</v>
       </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>53814</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>53816</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1405,334 +1401,334 @@
       <c r="D19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>53817</v>
       </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>53818</v>
       </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>53819</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>53820</v>
       </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>81</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>53821</v>
       </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>53822</v>
       </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>79</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>53823</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>76</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>53824</v>
       </c>
-      <c r="B27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>53825</v>
       </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29">
+    <row r="29" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>53826</v>
       </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A30">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>53827</v>
       </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A31">
+    <row r="31" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>53828</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32">
+    <row r="32" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>53829</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33">
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>53830</v>
       </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>53831</v>
       </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="B34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>53832</v>
       </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36">
+    <row r="36" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
         <v>53833</v>
       </c>
-      <c r="B36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A37">
+    <row r="37" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
         <v>53834</v>
       </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A38">
+    <row r="38" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
         <v>53835</v>
       </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>73</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>53836</v>
       </c>
@@ -1749,7 +1745,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>53837</v>
       </c>
@@ -1766,42 +1762,42 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
         <v>53840</v>
       </c>
-      <c r="B41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="6" t="s">
         <v>96</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A42">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
         <v>53842</v>
       </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="B42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>97</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43">
+    <row r="43" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
         <v>59833</v>
       </c>
       <c r="B43" t="s">
@@ -1817,139 +1813,139 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
         <v>59841</v>
       </c>
-      <c r="B44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>62080</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>164</v>
+      <c r="C45" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>60688</v>
       </c>
-      <c r="B46" t="s">
-        <v>167</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>166</v>
+      <c r="B46" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>161</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
         <v>60780</v>
       </c>
-      <c r="B47" t="s">
-        <v>167</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48">
+      <c r="B47" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
         <v>59692</v>
       </c>
-      <c r="B48" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>209</v>
+      <c r="B48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E48" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A49">
+        <v>194</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>59693</v>
       </c>
-      <c r="B49" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>210</v>
+      <c r="B49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="E49" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A50">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
         <v>59695</v>
       </c>
-      <c r="B50" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>208</v>
+      <c r="B50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E50" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A51">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
         <v>59696</v>
       </c>
-      <c r="B51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>211</v>
+      <c r="B51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E51" t="s">
-        <v>212</v>
+      <c r="E51" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E46:E48 E51">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1958,47 +1954,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F88D94-F9F2-4FF5-8669-E80BF5785B88}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>60532</v>
       </c>
       <c r="B2" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>175</v>
+      <c r="C2" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>118</v>
@@ -2007,140 +2003,170 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>60902</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>176</v>
+      <c r="C3" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>60903</v>
       </c>
       <c r="B4" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>175</v>
+      <c r="C4" s="9" t="s">
+        <v>168</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>60904</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>60905</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="12" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
         <v>60906</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>60908</v>
       </c>
       <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>177</v>
+        <v>138</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>60909</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>178</v>
+        <v>138</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="10" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>60910</v>
       </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="B10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="12" t="s">
         <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>59603</v>
+      </c>
+      <c r="B11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>59604</v>
+      </c>
+      <c r="B12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2153,84 +2179,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13F07D4-A043-4E09-992B-E3E60FFD6B6A}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>59007</v>
       </c>
       <c r="B2" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="9" t="s">
         <v>128</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>59006</v>
       </c>
       <c r="B3" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>59305</v>
       </c>
       <c r="B4" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="9" t="s">
         <v>121</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="10" t="s">
         <v>119</v>
       </c>
     </row>
@@ -2245,61 +2271,62 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>61353</v>
       </c>
-      <c r="B2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
         <v>60848</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9" t="s">
+      <c r="B3" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2311,334 +2338,238 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD268B07-DCAB-4CB2-B86B-FE38BE218C16}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>62551</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E2" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>62851</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>62852</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>62854</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>188</v>
+        <v>175</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="E5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>59716</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>59718</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>59720</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C8" t="s">
-        <v>185</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>188</v>
+        <v>175</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="E8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>53394</v>
       </c>
       <c r="B9" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>53395</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>200</v>
+        <v>188</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="E10" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>59542</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E11" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>59545</v>
       </c>
       <c r="B12" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>59551</v>
       </c>
       <c r="B13" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C13" t="s">
-        <v>185</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>188</v>
+        <v>175</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="E13" t="s">
-        <v>186</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>60684</v>
+      </c>
+      <c r="B14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="E15" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF729BDF-5E3F-45D9-877E-42F3FAFCFF40}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
-    <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="116" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>61353</v>
-      </c>
-      <c r="B2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>60848</v>
-      </c>
-      <c r="B3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="E3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>60851</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="E4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>60852</v>
-      </c>
-      <c r="E5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>60854</v>
-      </c>
-      <c r="E6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>60955</v>
-      </c>
-      <c r="E7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>61946</v>
-      </c>
-      <c r="E8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E3:E7">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
cambios en semilla de debinqr
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B253320F-A185-40F3-9232-F938394D20F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6FBCE8-9202-45C0-BC45-90AED18C6803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -683,7 +683,7 @@
     <t>"operacion_original":{"detalle":{"importe":1000},"qr_id_trx":"00000000000111111111111"},"objeto":{"ori_trx_id":"9223000000000066307"},"sql":"off"</t>
   </si>
   <si>
-    <t>"operacion_original":{"detalle":{"importe":1},"qr_id_trx":"Test%20Auto%2014594309"},"objeto":{"ori_trx_id":" "}},"sql":"off"</t>
+    <t>"operacion_original":{"detalle":{"importe":1},"qr_id_trx":"Test%20Auto%2014594309"},"objeto":{"ori_trx_id":" "},"sql":"off"</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -760,9 +760,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1944,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F88D94-F9F2-4FF5-8669-E80BF5785B88}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1981,7 +1978,7 @@
       <c r="B2" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="4" t="s">
         <v>168</v>
       </c>
       <c r="D2" s="2" t="s">

</xml_diff>

<commit_message>
cambios en cashout, semilla y archivo de excel
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB19F904-FFAB-4C92-9A14-6FF148649610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776C8D93-DF96-40EF-81E8-CBEA2D7E51FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR" sheetId="7" r:id="rId1"/>
@@ -413,15 +413,9 @@
     <t>CASHOUT - Validación ori_trx_id - CBU &gt; CBU</t>
   </si>
   <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta":{"codigo":"7552","descripcion":"O7L8GYKNXRV5MKONMPRZ50 - ID DE OPERACION  EXISTENTE"}}}</t>
-  </si>
-  <si>
     <t xml:space="preserve">CASHOUT - Validación ori_trx_id - CVU &gt; CVU </t>
   </si>
   <si>
-    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"7552","descripcion":"8PDX4OGNYJ0P80VN0L6EY5 - ID DE OPERACION  EXISTENTE"}}}</t>
-  </si>
-  <si>
     <t>"operacion":{"detalle":{ "tiempo_expiracion": 0}}</t>
   </si>
   <si>
@@ -692,25 +686,31 @@
     <t>"objeto":{"tipo":"CASHOUT"},"credito":{"cuit":"20956746117","banco":"000","sucursal":"0213","cuenta":{"cbu":"0000213699900070000000"},"titular":""},"debito":{"cuit":"20333048494","banco":"998","sucursal":"8851","cuenta":{"cbu":"9988851800000000000628"}},"importe":{"importe":10}}</t>
   </si>
   <si>
-    <t>"objeto":{"tipo":"CASHOUT","ori_trx_id":1126},"credito":{"cuit":"20000014479","banco":"000","sucursal":"8851","cuenta":{"cbu":"0000004800000000014485"},"titular":""},"debito":{"cuit":"27956331957","banco":"000","sucursal":"0161","cuenta":{"cbu":"0000161400000000004309"}},"importe":{"importe":10}}</t>
-  </si>
-  <si>
-    <t>"objeto":{"tipo":"CASHOUT","ori_trx_id":1141},"credito":{"cuit":"20333048494","banco":"998","sucursal":"8851","cuenta":{"cbu":"9988851800000000000628"},"titular":""},"debito":{"cuit":"20000009963","banco":"998","sucursal":"4788","cuenta":{"cbu":"9984788700000000000420"}},"importe":{"importe":10}}</t>
-  </si>
-  <si>
     <t>PaymentValidation</t>
   </si>
   <si>
     <t>"producto":"paymentvalidation"|"producto":"payment"</t>
   </si>
   <si>
-    <t>producto:"paymentvalidation"</t>
-  </si>
-  <si>
     <t>{"StatusCode":200,"Mensaje":{"validation_status":{"status":"PASS"}}}</t>
   </si>
   <si>
     <t>IdBilletera BCRA - Coelsa Aceptador - Payments/validations - OK</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta":{"codigo":"7552","descripcion":"8PDX4OGNYJ0PKMYN0L6EY5 - ID DE OPERACION  EXISTENTE"}}}</t>
+  </si>
+  <si>
+    <t>"objeto":{"tipo":"CASHOUT","ori_trx_id":1126},"credito":{"cuit":"20000014479","banco":"000","sucursal":"0004","cuenta":{"cbu":"0000004800000000014485"},"titular":""},"debito":{"cuit":"27956331957","banco":"000","sucursal":"0161","cuenta":{"cbu":"0000161400000000004309"}},"importe":{"importe":10}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":200,"Mensaje":{"respuesta": {"codigo":"7552","descripcion":"KLOEJWV9J0M3VO32QMD0GZ - ID DE OPERACION  EXISTENTE"}}}</t>
+  </si>
+  <si>
+    <t>"producto":"paymentvalidation"</t>
+  </si>
+  <si>
+    <t>"objeto":{"ori_trx_id":1141},"credito":{"cuit":"20333048494","banco":"998","sucursal":"8851","cuenta":{"cbu":"9988851800000000000628"},"titular":""},"debito":{"cuit":"20000009963","banco":"998","sucursal":"4788","cuenta":{"cbu":"9984788700000000000420"},"titular":""},"concepto":"VAR","importe":{"importe":10}}</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1173,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
@@ -1190,7 +1190,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
@@ -1207,7 +1207,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -1224,7 +1224,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -1258,7 +1258,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
@@ -1275,7 +1275,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>20</v>
@@ -1292,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -1598,7 +1598,7 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>51</v>
@@ -1853,13 +1853,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1867,13 +1867,13 @@
         <v>60688</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E46" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1881,13 +1881,13 @@
         <v>60780</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E47" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1898,13 +1898,13 @@
         <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E48" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1915,13 +1915,13 @@
         <v>5</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E49" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1932,13 +1932,13 @@
         <v>5</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1949,13 +1949,13 @@
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E51" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2009,7 +2009,7 @@
         <v>117</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>118</v>
@@ -2026,13 +2026,13 @@
         <v>117</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2043,13 +2043,13 @@
         <v>117</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>118</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2057,16 +2057,16 @@
         <v>60904</v>
       </c>
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" t="s">
         <v>136</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2074,16 +2074,16 @@
         <v>60905</v>
       </c>
       <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>137</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2091,16 +2091,16 @@
         <v>60906</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>118</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2108,16 +2108,16 @@
         <v>60908</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2125,16 +2125,16 @@
         <v>60909</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2142,16 +2142,16 @@
         <v>60910</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2159,14 +2159,14 @@
         <v>59603</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2174,14 +2174,14 @@
         <v>59604</v>
       </c>
       <c r="B12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2194,8 +2194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13F07D4-A043-4E09-992B-E3E60FFD6B6A}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,13 +2232,13 @@
         <v>121</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>125</v>
+        <v>220</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2249,10 +2249,10 @@
         <v>121</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>218</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>122</v>
@@ -2266,7 +2266,7 @@
         <v>121</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>120</v>
@@ -2320,16 +2320,16 @@
         <v>61353</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2337,14 +2337,14 @@
         <v>60848</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2352,16 +2352,16 @@
         <v>59844</v>
       </c>
       <c r="B4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>211</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2369,16 +2369,16 @@
         <v>59930</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2391,7 +2391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD268B07-DCAB-4CB2-B86B-FE38BE218C16}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -2426,14 +2426,14 @@
         <v>62551</v>
       </c>
       <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
         <v>162</v>
-      </c>
-      <c r="C2" t="s">
-        <v>164</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2441,13 +2441,13 @@
         <v>62851</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2455,13 +2455,13 @@
         <v>62852</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2469,16 +2469,16 @@
         <v>62854</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2486,13 +2486,13 @@
         <v>59716</v>
       </c>
       <c r="B6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" t="s">
         <v>177</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E6" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2500,13 +2500,13 @@
         <v>59718</v>
       </c>
       <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" t="s">
         <v>178</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2514,16 +2514,16 @@
         <v>59720</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2531,13 +2531,13 @@
         <v>53394</v>
       </c>
       <c r="B9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" t="s">
         <v>182</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E9" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2545,13 +2545,13 @@
         <v>53395</v>
       </c>
       <c r="B10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>187</v>
-      </c>
       <c r="E10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2559,13 +2559,13 @@
         <v>59542</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2573,13 +2573,13 @@
         <v>59545</v>
       </c>
       <c r="B12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2587,16 +2587,16 @@
         <v>59551</v>
       </c>
       <c r="B13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2604,19 +2604,19 @@
         <v>60684</v>
       </c>
       <c r="B14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="E15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mas casos de refunds
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F5B645-D7DD-4A16-A558-38B82C43E24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F1DB3D-73A5-4173-8B97-8B353647E79D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,15 +16,17 @@
     <sheet name="QR" sheetId="7" r:id="rId1"/>
     <sheet name="CONTRACARGOQR" sheetId="8" r:id="rId2"/>
     <sheet name="CASHOUT" sheetId="9" r:id="rId3"/>
-    <sheet name="INTEROPERBILIDAD" sheetId="12" r:id="rId4"/>
-    <sheet name="GETs" sheetId="13" r:id="rId5"/>
+    <sheet name="PAYMENTS" sheetId="12" r:id="rId4"/>
+    <sheet name="REFUNDS" sheetId="14" r:id="rId5"/>
+    <sheet name="GETs" sheetId="13" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CASHOUT!$A$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CONTRACARGOQR!$A$1:$E$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">GETs!$A$1:$E$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">INTEROPERBILIDAD!$A$1:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">GETs!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PAYMENTS!$A$1:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">QR!$A$1:$E$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">REFUNDS!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="266">
   <si>
     <t>Parametros</t>
   </si>
@@ -704,9 +706,6 @@
     <t>"objeto":{"ori_trx_id":1141},"credito":{"cuit":"20333048494","banco":"998","sucursal":"8851","cuenta":{"cbu":"9988851800000000000628"},"titular":""},"debito":{"cuit":"20000009963","banco":"998","sucursal":"4788","cuenta":{"cbu":"9984788700000000000420"},"titular":""},"concepto":"VAR","importe":{"importe":10}}</t>
   </si>
   <si>
-    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"producto":"refundvalidation"|"producto":"refund"</t>
-  </si>
-  <si>
     <t>IdBilletera BCRA - Coelsa Billetera Reverso - Refund/validations - OK</t>
   </si>
   <si>
@@ -756,6 +755,93 @@
   </si>
   <si>
     <t>{"StatusCode":400,"Mensaje":{"errors": [{"code":"Error","description":"bcra_id must be numeric"}]}}</t>
+  </si>
+  <si>
+    <t>PaymentValidation*-&gt;Payment*</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Aceptador - Payment - bcra_id - menor a 5 caracteres</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Aceptador - Payment - bcra_id - mayor a 5 caracteres</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Aceptador - Payment - bcra_id - alfanumérico</t>
+  </si>
+  <si>
+    <t>"payer":{"wallet":{"bcra_id":"01010"}}}|"payer":{"wallet":{"bcra_id":"0000"}}}</t>
+  </si>
+  <si>
+    <t>"payer":{"wallet":{"bcra_id":"01010"}}}|"payer":{"wallet":{"bcra_id":"000006"}}}</t>
+  </si>
+  <si>
+    <t>"payer":{"wallet":{"bcra_id":"01010"}}}|"payer":{"wallet":{"bcra_id":"a0b06"}}}</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Aceptador - Payment - bcra_id - vacío/null</t>
+  </si>
+  <si>
+    <t>"payer":{"wallet":{"bcra_id":"01010"}}}|"payer":{"wallet":{"bcra_id":" "}}}</t>
+  </si>
+  <si>
+    <t>"payer":{"wallet":{"bcra_id":"01010"}}}|"payer":{"wallet":{"bcra_id":"05050"}}}</t>
+  </si>
+  <si>
+    <t>{"StatusCode":201,"Mensaje":{"transaction": {"code":"REJECTED","description":"DATOS_INCONSISTENTES"}}}</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Aceptador  - Circuito Completo - Distinto bcra_id enviado en payments/validations y payments</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}</t>
+  </si>
+  <si>
+    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;RefundValidation*</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"payer":{"wallet":{"bcra_id":"0005"}}}</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Billetera - Refunds/Validations - bcra_id - menor a 5 caracteres</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"payer":{"wallet":{"bcra_id":"000505"}}}</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Billetera - Refunds/Validations - bcra_id - mayor a 5 caracteres</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Billetera - Refunds/Validations - bcra_id - alfanumérico</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"payer":{"wallet":{"bcra_id":"a0b06"}}}</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Billetera - Refunds/Validations - bcra_id - vacío/null</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"payer":{"wallet":{"bcra_id":" "}}}</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Billetera - Refunds - bcra_id - menor a 5 caracteres</t>
+  </si>
+  <si>
+    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;RefundValidation*-&gt;Refund*</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"payer":{"wallet":{"bcra_id":"05050"}}}|"payer":{"wallet":{"bcra_id":"0505"}}}</t>
+  </si>
+  <si>
+    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"payer":{"wallet":{"bcra_id":"05050"}}}|"payer":{"wallet":{"bcra_id":"050505"}}}</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Billetera - Refunds - bcra_id - mayor a 5 caracteres</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Billetera - Refunds - bcra_id - alfanumérico</t>
+  </si>
+  <si>
+    <t>IdBilletera BCRA - Coelsa Billetera - Refunds - bcra_id - vacío/null</t>
   </si>
 </sst>
 </file>
@@ -2351,16 +2437,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F27905B-1E87-40DF-B6B4-452FD9A02DC6}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
     <col min="4" max="4" width="82.42578125" customWidth="1"/>
     <col min="5" max="5" width="81.140625" customWidth="1"/>
@@ -2412,134 +2498,188 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>59844</v>
+        <v>59930</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>59930</v>
-      </c>
-      <c r="B5" t="s">
-        <v>213</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>60040</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>59950</v>
+        <v>59953</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>226</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
-        <v>60040</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>224</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>223</v>
+      <c r="A7">
+        <v>59956</v>
+      </c>
+      <c r="B7" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>59953</v>
+        <v>59957</v>
       </c>
       <c r="B8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>59986</v>
+      </c>
+      <c r="B9" t="s">
         <v>234</v>
       </c>
-      <c r="E8" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>59956</v>
-      </c>
-      <c r="B9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C9" t="s">
-        <v>228</v>
+      <c r="C9" s="11" t="s">
+        <v>231</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E9" t="s">
-        <v>229</v>
+        <v>233</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>59957</v>
+        <v>59970</v>
       </c>
       <c r="B10" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C10" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>59971</v>
+      </c>
+      <c r="B11" t="s">
         <v>237</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
-        <v>59986</v>
-      </c>
-      <c r="B11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>232</v>
+      <c r="C11" t="s">
+        <v>242</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E11" s="11" t="s">
         <v>233</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>59984</v>
+      </c>
+      <c r="B12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>59987</v>
+      </c>
+      <c r="B13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>60386</v>
+      </c>
+      <c r="B14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2549,6 +2689,213 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFA3C39-F395-444B-9CEE-CFC2FA04FF9A}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="100" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="81.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>59844</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>59950</v>
+      </c>
+      <c r="B3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>59991</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>59993</v>
+      </c>
+      <c r="B5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>59994</v>
+      </c>
+      <c r="B6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>59997</v>
+      </c>
+      <c r="B7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>59998</v>
+      </c>
+      <c r="B8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>59999</v>
+      </c>
+      <c r="B9" t="s">
+        <v>260</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>60002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>60003</v>
+      </c>
+      <c r="B11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD268B07-DCAB-4CB2-B86B-FE38BE218C16}">
   <dimension ref="A1:E15"/>
   <sheetViews>

</xml_diff>

<commit_message>
Validacion de paymentvalidation y payment
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F5B645-D7DD-4A16-A558-38B82C43E24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5C7E01-3BA8-4BB1-B8E9-9276D43F40D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR" sheetId="7" r:id="rId1"/>
@@ -809,7 +809,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -834,19 +834,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1156,16 +1143,16 @@
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1182,7 +1169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>53766</v>
       </c>
@@ -1199,7 +1186,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>53799</v>
       </c>
@@ -1216,7 +1203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>53800</v>
       </c>
@@ -1233,7 +1220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>53801</v>
       </c>
@@ -1250,7 +1237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>53802</v>
       </c>
@@ -1267,7 +1254,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>53803</v>
       </c>
@@ -1284,7 +1271,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>53804</v>
       </c>
@@ -1301,7 +1288,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>53805</v>
       </c>
@@ -1318,7 +1305,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>53806</v>
       </c>
@@ -1335,7 +1322,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>53807</v>
       </c>
@@ -1352,7 +1339,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>53808</v>
       </c>
@@ -1369,7 +1356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>53809</v>
       </c>
@@ -1386,7 +1373,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>53810</v>
       </c>
@@ -1403,7 +1390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>53811</v>
       </c>
@@ -1420,7 +1407,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>53812</v>
       </c>
@@ -1437,7 +1424,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>53813</v>
       </c>
@@ -1454,7 +1441,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>53814</v>
       </c>
@@ -1471,7 +1458,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>53816</v>
       </c>
@@ -1488,7 +1475,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>53817</v>
       </c>
@@ -1505,7 +1492,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>53818</v>
       </c>
@@ -1522,7 +1509,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>53819</v>
       </c>
@@ -1539,7 +1526,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>53820</v>
       </c>
@@ -1556,7 +1543,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>53821</v>
       </c>
@@ -1573,7 +1560,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>53822</v>
       </c>
@@ -1590,7 +1577,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>53823</v>
       </c>
@@ -1607,7 +1594,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>53824</v>
       </c>
@@ -1624,7 +1611,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>53825</v>
       </c>
@@ -1641,7 +1628,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>53826</v>
       </c>
@@ -1658,7 +1645,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>53827</v>
       </c>
@@ -1675,7 +1662,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>53828</v>
       </c>
@@ -1692,7 +1679,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>53829</v>
       </c>
@@ -1709,7 +1696,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>53830</v>
       </c>
@@ -1726,7 +1713,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>53831</v>
       </c>
@@ -1743,7 +1730,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>53832</v>
       </c>
@@ -1760,7 +1747,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>53833</v>
       </c>
@@ -1777,7 +1764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>53834</v>
       </c>
@@ -1794,7 +1781,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>53835</v>
       </c>
@@ -1811,7 +1798,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>53836</v>
       </c>
@@ -1828,7 +1815,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>53837</v>
       </c>
@@ -1845,7 +1832,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>53840</v>
       </c>
@@ -1862,7 +1849,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>53842</v>
       </c>
@@ -1879,7 +1866,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>59833</v>
       </c>
@@ -1896,7 +1883,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>59841</v>
       </c>
@@ -1913,7 +1900,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>62080</v>
       </c>
@@ -1930,7 +1917,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>60688</v>
       </c>
@@ -1944,7 +1931,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>60780</v>
       </c>
@@ -1958,7 +1945,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>59692</v>
       </c>
@@ -1975,7 +1962,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>59693</v>
       </c>
@@ -1992,7 +1979,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>59695</v>
       </c>
@@ -2009,7 +1996,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>59696</v>
       </c>
@@ -2043,16 +2030,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2069,14 +2056,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>60532</v>
       </c>
       <c r="B2" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -2086,7 +2073,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>60902</v>
       </c>
@@ -2103,7 +2090,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>60903</v>
       </c>
@@ -2120,7 +2107,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>60904</v>
       </c>
@@ -2137,7 +2124,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>60905</v>
       </c>
@@ -2154,7 +2141,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>60906</v>
       </c>
@@ -2171,7 +2158,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>60908</v>
       </c>
@@ -2188,7 +2175,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>60909</v>
       </c>
@@ -2205,7 +2192,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>60910</v>
       </c>
@@ -2222,7 +2209,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>59603</v>
       </c>
@@ -2237,7 +2224,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>59604</v>
       </c>
@@ -2266,16 +2253,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2292,7 +2279,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>59007</v>
       </c>
@@ -2309,7 +2296,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>59006</v>
       </c>
@@ -2326,7 +2313,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>59305</v>
       </c>
@@ -2353,20 +2340,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F27905B-1E87-40DF-B6B4-452FD9A02DC6}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="53.26953125" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="81.140625" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="81.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2383,7 +2370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>61353</v>
       </c>
@@ -2397,22 +2384,22 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>60848</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>59844</v>
       </c>
@@ -2429,7 +2416,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>59930</v>
       </c>
@@ -2443,7 +2430,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>59950</v>
       </c>
@@ -2457,24 +2444,24 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
         <v>60040</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="12" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>59953</v>
       </c>
@@ -2491,7 +2478,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>59956</v>
       </c>
@@ -2508,7 +2495,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>59957</v>
       </c>
@@ -2525,20 +2512,20 @@
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11">
         <v>59986</v>
       </c>
       <c r="B11" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" t="s">
         <v>232</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" t="s">
         <v>233</v>
       </c>
     </row>
@@ -2552,20 +2539,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD268B07-DCAB-4CB2-B86B-FE38BE218C16}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="29.1796875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.42578125" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="82.453125" customWidth="1"/>
+    <col min="5" max="5" width="58.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2582,7 +2569,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>62551</v>
       </c>
@@ -2597,7 +2584,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>62851</v>
       </c>
@@ -2611,7 +2598,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>62852</v>
       </c>
@@ -2625,7 +2612,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>62854</v>
       </c>
@@ -2642,7 +2629,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>59716</v>
       </c>
@@ -2656,7 +2643,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>59718</v>
       </c>
@@ -2670,7 +2657,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>59720</v>
       </c>
@@ -2687,7 +2674,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>53394</v>
       </c>
@@ -2701,7 +2688,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>53395</v>
       </c>
@@ -2715,7 +2702,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>59542</v>
       </c>
@@ -2729,7 +2716,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>59545</v>
       </c>
@@ -2743,7 +2730,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>59551</v>
       </c>
@@ -2760,7 +2747,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>60684</v>
       </c>
@@ -2774,7 +2761,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="E15" t="s">
         <v>205</v>

</xml_diff>

<commit_message>
Cambios payment, paymentvalidation y contracargoqr
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645F36AA-4C5C-456A-98A2-414AF4512C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E536F7-5DD1-4A00-B253-465868AC0BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -898,10 +898,10 @@
     <t>"operacion_original":{"detalle":{"importe":10},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}|"operacion_original":{"detalle":{"importe":10},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}</t>
   </si>
   <si>
-    <t>PaymentValidation-&gt;Payment-&gt;QRSolicitudContraCargoPayment*</t>
-  </si>
-  <si>
-    <t>"banco":"016","operacion_original":{"detalle":{"importe":10.0},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}</t>
+    <t>"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":10.0},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}</t>
+  </si>
+  <si>
+    <t>PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*</t>
   </si>
 </sst>
 </file>
@@ -2172,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F88D94-F9F2-4FF5-8669-E80BF5785B88}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2407,10 +2407,10 @@
         <v>60040</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" s="11" t="s">
         <v>284</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>285</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
get debinid, debin2, debin3, debin4, debin5
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7B7A11-3DE2-4207-A492-A05B5CF4AE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CDFE0B-E4E1-4C14-B69C-465F806C1A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR" sheetId="7" r:id="rId1"/>
@@ -883,22 +883,22 @@
     <t>PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*</t>
   </si>
   <si>
+    <t>PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*-&gt;QRSolicitudContraCargoPayment*</t>
+  </si>
+  <si>
+    <t>PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*-&gt;PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*</t>
+  </si>
+  <si>
     <t>"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}</t>
   </si>
   <si>
-    <t>PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*-&gt;QRSolicitudContraCargoPayment*</t>
-  </si>
-  <si>
-    <t>PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*-&gt;PaymentValidation*-&gt;Payment*-&gt;QRSolicitudContraCargoPayment*</t>
-  </si>
-  <si>
     <t>"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":10.0},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}|"banco":"016","operacion_original":{"detalle":{"importe":10.0},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}},"objeto":{"ori_trx_id":"nuevo"}</t>
   </si>
   <si>
     <t>"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}|"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}</t>
   </si>
   <si>
-    <t>"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":10},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}|"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":10},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}}</t>
+    <t>"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}|"banco":"902"|"banco":"902"|"banco":"016","operacion_original":{"detalle":{"importe":1000},"vendedor":{"cuit":"20374372689","cbu":"0000084000000000000024"}}</t>
   </si>
 </sst>
 </file>
@@ -914,7 +914,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -930,12 +930,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -973,20 +967,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1286,16 +1280,16 @@
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1312,7 +1306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>53766</v>
       </c>
@@ -1329,7 +1323,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>53799</v>
       </c>
@@ -1346,7 +1340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>53800</v>
       </c>
@@ -1363,7 +1357,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>53801</v>
       </c>
@@ -1380,7 +1374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>53802</v>
       </c>
@@ -1397,7 +1391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>53803</v>
       </c>
@@ -1414,7 +1408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>53804</v>
       </c>
@@ -1431,7 +1425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>53805</v>
       </c>
@@ -1448,7 +1442,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>53806</v>
       </c>
@@ -1465,7 +1459,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>53807</v>
       </c>
@@ -1482,7 +1476,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>53808</v>
       </c>
@@ -1499,7 +1493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>53809</v>
       </c>
@@ -1516,7 +1510,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>53810</v>
       </c>
@@ -1533,7 +1527,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>53811</v>
       </c>
@@ -1550,7 +1544,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>53812</v>
       </c>
@@ -1567,7 +1561,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>53813</v>
       </c>
@@ -1584,7 +1578,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>53814</v>
       </c>
@@ -1601,7 +1595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>53816</v>
       </c>
@@ -1618,7 +1612,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>53817</v>
       </c>
@@ -1635,7 +1629,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>53818</v>
       </c>
@@ -1652,7 +1646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>53819</v>
       </c>
@@ -1669,7 +1663,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>53820</v>
       </c>
@@ -1686,7 +1680,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>53821</v>
       </c>
@@ -1703,7 +1697,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>53822</v>
       </c>
@@ -1720,7 +1714,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>53823</v>
       </c>
@@ -1737,7 +1731,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>53824</v>
       </c>
@@ -1754,7 +1748,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>53825</v>
       </c>
@@ -1771,7 +1765,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>53826</v>
       </c>
@@ -1788,7 +1782,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>53827</v>
       </c>
@@ -1805,7 +1799,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>53828</v>
       </c>
@@ -1822,7 +1816,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>53829</v>
       </c>
@@ -1839,7 +1833,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>53830</v>
       </c>
@@ -1856,7 +1850,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>53831</v>
       </c>
@@ -1873,7 +1867,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>53832</v>
       </c>
@@ -1890,7 +1884,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>53833</v>
       </c>
@@ -1907,7 +1901,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>53834</v>
       </c>
@@ -1924,7 +1918,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>53835</v>
       </c>
@@ -1941,7 +1935,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>53836</v>
       </c>
@@ -1958,7 +1952,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>53837</v>
       </c>
@@ -1975,7 +1969,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>53840</v>
       </c>
@@ -1992,7 +1986,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>53842</v>
       </c>
@@ -2009,7 +2003,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>59833</v>
       </c>
@@ -2026,7 +2020,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>59841</v>
       </c>
@@ -2043,7 +2037,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>62080</v>
       </c>
@@ -2060,7 +2054,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>60688</v>
       </c>
@@ -2074,7 +2068,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>60780</v>
       </c>
@@ -2088,7 +2082,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>59692</v>
       </c>
@@ -2105,7 +2099,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>59693</v>
       </c>
@@ -2122,7 +2116,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>59695</v>
       </c>
@@ -2139,7 +2133,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>59696</v>
       </c>
@@ -2169,20 +2163,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F88D94-F9F2-4FF5-8669-E80BF5785B88}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="98.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="98.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2199,7 +2193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>60532</v>
       </c>
@@ -2216,7 +2210,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>60902</v>
       </c>
@@ -2233,7 +2227,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>60903</v>
       </c>
@@ -2250,7 +2244,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>60904</v>
       </c>
@@ -2267,7 +2261,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>60905</v>
       </c>
@@ -2284,7 +2278,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>60906</v>
       </c>
@@ -2301,7 +2295,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>60908</v>
       </c>
@@ -2318,7 +2312,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>60909</v>
       </c>
@@ -2335,7 +2329,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>60910</v>
       </c>
@@ -2352,7 +2346,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>59603</v>
       </c>
@@ -2367,7 +2361,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>59604</v>
       </c>
@@ -2382,109 +2376,109 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>60256</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="8" t="s">
         <v>268</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="9" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="8">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>60040</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="10" t="s">
         <v>278</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="13" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>60268</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>60271</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>60274</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>282</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="C17" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="8">
-        <v>60271</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>279</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="8">
-        <v>60274</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="C17" s="11" t="s">
+      <c r="E17" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>60347</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="8">
-        <v>60347</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="6" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>60349</v>
       </c>
@@ -2511,20 +2505,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C13F07D4-A043-4E09-992B-E3E60FFD6B6A}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2541,7 +2535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>59007</v>
       </c>
@@ -2558,7 +2552,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>59006</v>
       </c>
@@ -2575,7 +2569,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>59305</v>
       </c>
@@ -2606,16 +2600,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="54.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="81.1796875" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2632,7 +2626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>61353</v>
       </c>
@@ -2646,7 +2640,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>60848</v>
       </c>
@@ -2661,7 +2655,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>59930</v>
       </c>
@@ -2675,7 +2669,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>59953</v>
       </c>
@@ -2692,7 +2686,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>59956</v>
       </c>
@@ -2709,7 +2703,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>59957</v>
       </c>
@@ -2726,7 +2720,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>59986</v>
       </c>
@@ -2743,7 +2737,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>59970</v>
       </c>
@@ -2760,7 +2754,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>59971</v>
       </c>
@@ -2777,7 +2771,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>59984</v>
       </c>
@@ -2794,7 +2788,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>59987</v>
       </c>
@@ -2811,7 +2805,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>60386</v>
       </c>
@@ -2828,7 +2822,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
     </row>
   </sheetData>
@@ -2845,16 +2839,16 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="54.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="81.1796875" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2871,7 +2865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>59844</v>
       </c>
@@ -2888,7 +2882,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>59950</v>
       </c>
@@ -2902,7 +2896,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>59991</v>
       </c>
@@ -2919,7 +2913,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>59993</v>
       </c>
@@ -2936,7 +2930,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>59994</v>
       </c>
@@ -2953,7 +2947,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>59997</v>
       </c>
@@ -2970,7 +2964,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>59998</v>
       </c>
@@ -2987,7 +2981,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>59999</v>
       </c>
@@ -3004,7 +2998,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>60002</v>
       </c>
@@ -3021,7 +3015,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>60003</v>
       </c>
@@ -3038,7 +3032,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>60246</v>
       </c>
@@ -3067,16 +3061,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="29.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
-    <col min="4" max="4" width="82.453125" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" customWidth="1"/>
+    <col min="4" max="4" width="82.42578125" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3093,7 +3087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>62551</v>
       </c>
@@ -3108,7 +3102,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>62851</v>
       </c>
@@ -3122,7 +3116,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>62852</v>
       </c>
@@ -3136,7 +3130,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>62854</v>
       </c>
@@ -3153,7 +3147,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>59716</v>
       </c>
@@ -3167,7 +3161,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>59718</v>
       </c>
@@ -3181,7 +3175,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>59720</v>
       </c>
@@ -3198,7 +3192,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>53394</v>
       </c>
@@ -3212,7 +3206,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>53395</v>
       </c>
@@ -3226,7 +3220,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>59542</v>
       </c>
@@ -3240,7 +3234,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>59545</v>
       </c>
@@ -3254,7 +3248,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>59551</v>
       </c>
@@ -3271,7 +3265,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60684</v>
       </c>
@@ -3285,7 +3279,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="E15" t="s">
         <v>204</v>

</xml_diff>

<commit_message>
TCs TRX3.0 - REFUNDS OK
</commit_message>
<xml_diff>
--- a/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
+++ b/Ambiente/Debin - QR - Escenarios y Casos de Pruebas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Katalon Studio\Inazuma 3 - Debin\Ambiente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4478E5E8-B30C-4BD4-94E5-86418C2AA82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F6EC29-5059-41A6-92D2-35FB45227701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">GETs!$A$1:$E$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PAYMENTS!$A$1:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">QR!$A$1:$E$45</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">REFUNDS!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">REFUNDS!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="336">
   <si>
     <t>Parametros</t>
   </si>
@@ -784,12 +784,6 @@
     <t>"operacion":{"detalle":{"importe":1000}}}|"operacion":{"comprador":{"cuit":"23000009989","cuenta":{"cbu":"9985340400000000000529"}},"detalle":{"ori_terminal":"","ori_adicional":"","moneda":"032","importe":1000}}}|"operacion_original":{"detalle":{"importe":1}}}|"operacion_original":{"detalle":{"importe":1}},"objeto":{"ori_trx_id":"nuevo"}|"operacion_original":{"detalle":{"importe":1}},"objeto":{"ori_trx_id":"nuevo"}</t>
   </si>
   <si>
-    <t>QRDebin*-&gt;ConfirmaDebito*-&gt;RefundValidation-&gt;Refund-&gt;Aviso*</t>
-  </si>
-  <si>
-    <t>"operacion":{"detalle":{"importe":1000,"qr":"00020101021143160012com.todopago44110007com.agr48260012com.todopago010627571950150011309598932565204970053030325802AR5922Jordan Empresa Preprod6013VILLA URQUIZA6304d9da","id_billetera":4}}}|"operacion":{"detalle":{"importe":1000}}}|"id":"debin.id","aviso":"QROperacionFinalizada","producto":"responder"</t>
-  </si>
-  <si>
     <t>Coelsa Billetera - Refund - Aviso QROperaciónFinalizada IDHASH de la operación original - OK</t>
   </si>
   <si>
@@ -1052,6 +1046,12 @@
   </si>
   <si>
     <t xml:space="preserve">Debin QR - NO interoperable --&gt; Comercio Inexistente </t>
+  </si>
+  <si>
+    <t>PaymentValidationbcra*</t>
+  </si>
+  <si>
+    <t>PaymentValidationbcra*-&gt;Paymentbcra*</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63218BCB-F1F0-4D18-A551-3DB8181D382F}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B66" workbookViewId="0">
+    <sheetView topLeftCell="B66" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
@@ -1503,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>95</v>
@@ -1673,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>22</v>
@@ -1792,7 +1792,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>31</v>
@@ -1809,13 +1809,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1928,7 +1928,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>43</v>
@@ -1945,7 +1945,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>45</v>
@@ -1996,7 +1996,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>50</v>
@@ -2013,10 +2013,10 @@
         <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E32" t="s">
         <v>52</v>
@@ -2030,7 +2030,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>53</v>
@@ -2047,7 +2047,7 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>53</v>
@@ -2149,10 +2149,10 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E40" t="s">
         <v>101</v>
@@ -2293,13 +2293,13 @@
         <v>59692</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E49" s="10" t="s">
         <v>178</v>
@@ -2310,13 +2310,13 @@
         <v>59693</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C50" s="16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>177</v>
@@ -2327,10 +2327,10 @@
         <v>59695</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>62</v>
@@ -2344,10 +2344,10 @@
         <v>59696</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>62</v>
@@ -2361,16 +2361,16 @@
         <v>60874</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" spans="1:5" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2378,16 +2378,16 @@
         <v>60875</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E54" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:5" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2395,16 +2395,16 @@
         <v>60876</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2412,16 +2412,16 @@
         <v>60879</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E56" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2429,16 +2429,16 @@
         <v>60880</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E57" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2446,16 +2446,16 @@
         <v>60882</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D58" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E58" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2463,16 +2463,16 @@
         <v>60946</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D59" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:5" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2480,16 +2480,16 @@
         <v>60947</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2497,14 +2497,14 @@
         <v>62909</v>
       </c>
       <c r="B61" t="s">
+        <v>266</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2515,13 +2515,13 @@
         <v>5</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2529,13 +2529,13 @@
         <v>62914</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E63" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2546,13 +2546,13 @@
         <v>5</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E64" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2563,13 +2563,13 @@
         <v>5</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D65" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E65" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2580,13 +2580,13 @@
         <v>5</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E66" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="67" spans="1:5" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -2597,13 +2597,13 @@
         <v>5</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2614,13 +2614,13 @@
         <v>5</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>62</v>
       </c>
       <c r="E68" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2628,14 +2628,14 @@
         <v>53711</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D69" s="12"/>
       <c r="E69" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2646,13 +2646,13 @@
         <v>5</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2663,13 +2663,13 @@
         <v>5</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,7 +2680,7 @@
         <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2691,7 +2691,7 @@
         <v>5</v>
       </c>
       <c r="E73" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2931,16 +2931,16 @@
         <v>60256</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>109</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2948,10 +2948,10 @@
         <v>60040</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>109</v>
@@ -2965,16 +2965,16 @@
         <v>60268</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2982,16 +2982,16 @@
         <v>60271</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2999,16 +2999,16 @@
         <v>60274</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>109</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3016,16 +3016,16 @@
         <v>60347</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3033,16 +3033,16 @@
         <v>60349</v>
       </c>
       <c r="B19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>124</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3147,7 +3147,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,71 +3219,71 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>59953</v>
       </c>
-      <c r="B5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="9" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>59956</v>
       </c>
-      <c r="B6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="9" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>59957</v>
       </c>
-      <c r="B7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="9" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:5" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>59986</v>
       </c>
-      <c r="B8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -3292,7 +3292,7 @@
         <v>59970</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>335</v>
       </c>
       <c r="C9" t="s">
         <v>218</v>
@@ -3380,13 +3380,13 @@
         <v>212</v>
       </c>
       <c r="C14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>196</v>
       </c>
       <c r="E14" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3399,8 +3399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCFA3C39-F395-444B-9CEE-CFC2FA04FF9A}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3567,7 +3567,7 @@
         <v>60002</v>
       </c>
       <c r="B10" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>233</v>
@@ -3587,7 +3587,7 @@
         <v>237</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>211</v>
@@ -3596,19 +3596,21 @@
         <v>242</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>60246</v>
       </c>
       <c r="B12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>246</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="5" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>